<commit_message>
Update - Ledger Kelas
</commit_message>
<xml_diff>
--- a/public/template/Template Jurnal.xlsx
+++ b/public/template/Template Jurnal.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\xampp\htdocs\annahl\public\template\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{37E75A8F-1B84-4923-B92D-ED022EEAE18B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B13B879F-27A9-452D-A60D-1DFDBFF50E79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Kompetensi</t>
   </si>
@@ -40,6 +40,9 @@
   </si>
   <si>
     <t>Materi</t>
+  </si>
+  <si>
+    <t>Pengganti</t>
   </si>
 </sst>
 </file>
@@ -86,7 +89,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -124,18 +127,30 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="164" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
@@ -148,9 +163,17 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="164" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -431,53 +454,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:F1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.7109375" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.140625" style="4"/>
-    <col min="3" max="3" width="9.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.7109375" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.140625" style="3"/>
+    <col min="3" max="3" width="9.85546875" style="3" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="11.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="10.140625" style="1" customWidth="1"/>
+    <col min="6" max="6" width="9.85546875" style="8" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:6" s="10" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="6" t="s">
+      <c r="D1" s="5" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="7" t="s">
         <v>4</v>
       </c>
+      <c r="F1" s="9" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
-  <sheetProtection algorithmName="SHA-512" hashValue="XOSxIn2irUkYPwcfEm4O0gtgjPZ1Tnx3ppBWaDGUQxWjIBx9BexFL7ZPeWq+UQmOEeXD5E7/dv9mfZypXiofeA==" saltValue="3zHsi8xyt8rtx2i8Aws4sg==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1"/>
+  <sheetProtection algorithmName="SHA-512" hashValue="SGWKiTVQyR3nBuDX9TzBUBf8C9rlgFJnmyq3ltxSdNaUVUGFsAP3lD/WB0w7dyM0dNcTA8n+NcaTxa57GyKp+g==" saltValue="Pfcwih0JnUbORkqHziqVqw==" spinCount="100000" sheet="1" formatCells="0" formatColumns="0" formatRows="0" selectLockedCells="1"/>
   <phoneticPr fontId="2" type="noConversion"/>
-  <dataValidations count="4">
+  <dataValidations count="5">
     <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only date format allowed" promptTitle="Format" prompt="yyyy-mm-dd" sqref="A2:A1048576" xr:uid="{29D89CFD-7AB8-415C-B440-EC95327CBA53}">
       <formula1>35431</formula1>
     </dataValidation>
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="B1:B1048576" xr:uid="{633313F1-D624-4B78-AD06-699C510E2531}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only Number 1 - 4" prompt="Number between 1 - 4" sqref="C1:C1048576" xr:uid="{73E5584F-0A99-419A-AF86-7DCBA543904E}">
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Only Number 1 - 5" prompt="Number between 1 - 5" sqref="C2:C1048576" xr:uid="{73E5584F-0A99-419A-AF86-7DCBA543904E}">
       <formula1>1</formula1>
-      <formula2>4</formula2>
+      <formula2>5</formula2>
     </dataValidation>
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="3. or 4." sqref="D2:D1048576" xr:uid="{4BA93B9A-2DC6-43B6-A935-E20DB120BA45}"/>
+    <dataValidation type="whole" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Number 0 or 1" prompt="0 = No_x000a_1 = Yes" sqref="F1:F1048576" xr:uid="{0C6587B7-0884-4A78-8CB6-E37107772B56}">
+      <formula1>0</formula1>
+      <formula2>1</formula2>
+    </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>